<commit_message>
Added negative test cases and upgraded 'museum-api' package to 0.0.8
</commit_message>
<xml_diff>
--- a/reports/museum_data.xlsx
+++ b/reports/museum_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BR16"/>
+  <dimension ref="A1:BQ16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,477 +434,475 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>objectID</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>objectID</t>
+          <t>isHighlight</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>isHighlight</t>
+          <t>accessionNumber</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>accessionNumber</t>
+          <t>accessionYear</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>accessionYear</t>
+          <t>isPublicDomain</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>isPublicDomain</t>
+          <t>primaryImage</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>primaryImage</t>
+          <t>primaryImageSmall</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>primaryImageSmall</t>
+          <t>additionalImages</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>additionalImages</t>
+          <t>department</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>department</t>
+          <t>objectName</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>objectName</t>
+          <t>title</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>culture</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>culture</t>
+          <t>period</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>period</t>
+          <t>dynasty</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>dynasty</t>
+          <t>reign</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>reign</t>
+          <t>portfolio</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>portfolio</t>
+          <t>artistRole</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>artistRole</t>
+          <t>artistPrefix</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>artistPrefix</t>
+          <t>artistDisplayName</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>artistDisplayName</t>
+          <t>artistDisplayBio</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>artistDisplayBio</t>
+          <t>artistSuffix</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>artistSuffix</t>
+          <t>artistAlphaSort</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>artistAlphaSort</t>
+          <t>artistNationality</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>artistNationality</t>
+          <t>artistBeginDate</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>artistBeginDate</t>
+          <t>artistEndDate</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>artistEndDate</t>
+          <t>artistGender</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>artistGender</t>
+          <t>artistWikidata_URL</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>artistWikidata_URL</t>
+          <t>artistULAN_URL</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>artistULAN_URL</t>
+          <t>objectDate</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>objectDate</t>
+          <t>objectBeginDate</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>objectBeginDate</t>
+          <t>objectEndDate</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>objectEndDate</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>medium</t>
+          <t>dimensions</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>dimensions</t>
+          <t>measurements</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>measurements</t>
+          <t>creditLine</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>creditLine</t>
+          <t>geographyType</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>geographyType</t>
+          <t>city</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>city</t>
+          <t>state</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>state</t>
+          <t>county</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>county</t>
+          <t>country</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>country</t>
+          <t>region</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>subregion</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>subregion</t>
+          <t>locale</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>locale</t>
+          <t>locus</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>locus</t>
+          <t>excavation</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>excavation</t>
+          <t>river</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>classification</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>rightsAndReproduction</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>rightsAndReproduction</t>
+          <t>linkResource</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
-          <t>linkResource</t>
+          <t>metadataDate</t>
         </is>
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>metadataDate</t>
+          <t>repository</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>repository</t>
+          <t>objectURL</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>objectURL</t>
+          <t>tags</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>tags</t>
+          <t>objectWikidata_URL</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>objectWikidata_URL</t>
+          <t>isTimelineWork</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
         <is>
-          <t>isTimelineWork</t>
+          <t>GalleryNumber</t>
         </is>
       </c>
       <c r="BE1" s="1" t="inlineStr">
         <is>
-          <t>GalleryNumber</t>
+          <t>constituentID</t>
         </is>
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
-          <t>constituentID</t>
+          <t>role</t>
         </is>
       </c>
       <c r="BG1" s="1" t="inlineStr">
         <is>
-          <t>role</t>
+          <t>name</t>
         </is>
       </c>
       <c r="BH1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>constituentULAN_URL</t>
         </is>
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>constituentULAN_URL</t>
+          <t>constituentWikidata_URL</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>constituentWikidata_URL</t>
+          <t>gender</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>gender</t>
+          <t>constituents</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>constituents</t>
+          <t>elementName</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>elementName</t>
+          <t>elementDescription</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>elementDescription</t>
+          <t>elementMeasurements</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>elementMeasurements</t>
+          <t>term</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>term</t>
+          <t>AAT_URL</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
-        <is>
-          <t>AAT_URL</t>
-        </is>
-      </c>
-      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>Wikidata_URL</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="b">
-        <v>0</v>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1979.486.1</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1979.486.1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
           <t>1979</t>
         </is>
       </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
           <t>One-dollar Liberty Head Coin</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>Maker</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>James Barton Longacre</t>
+        </is>
+      </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>James Barton Longacre</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
           <t>American, Delaware County, Pennsylvania 1794–1869 Philadelphia, Pennsylvania</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Longacre, James Barton</t>
+        </is>
+      </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Longacre, James Barton</t>
+          <t>American</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>American</t>
+          <t>1794</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>1794</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
           <t>1869</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>https://www.wikidata.org/wiki/Q3806459</t>
+        </is>
+      </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>https://www.wikidata.org/wiki/Q3806459</t>
+          <t>http://vocab.getty.edu/page/ulan/500011409</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500011409</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
           <t>1853</t>
         </is>
+      </c>
+      <c r="AD2" t="n">
+        <v>1853</v>
       </c>
       <c r="AE2" t="n">
         <v>1853</v>
       </c>
-      <c r="AF2" t="n">
-        <v>1853</v>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
           <t>Dimensions unavailable</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="inlineStr">
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr">
         <is>
           <t>Gift of Heinz L. Stoppelmann, 1979</t>
         </is>
       </c>
+      <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
@@ -918,51 +916,51 @@
       <c r="AU2" t="inlineStr"/>
       <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="inlineStr"/>
-      <c r="AX2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY2" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ2" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA2" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/1</t>
         </is>
       </c>
+      <c r="BA2" t="inlineStr"/>
       <c r="BB2" t="inlineStr"/>
-      <c r="BC2" t="inlineStr"/>
-      <c r="BD2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BE2" t="inlineStr"/>
-      <c r="BF2" t="n">
+      <c r="BC2" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="n">
         <v>164292</v>
       </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>Maker</t>
+        </is>
+      </c>
       <c r="BG2" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>James Barton Longacre</t>
         </is>
       </c>
       <c r="BH2" t="inlineStr">
         <is>
-          <t>James Barton Longacre</t>
+          <t>http://vocab.getty.edu/page/ulan/500011409</t>
         </is>
       </c>
       <c r="BI2" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500011409</t>
-        </is>
-      </c>
-      <c r="BJ2" t="inlineStr">
-        <is>
           <t>https://www.wikidata.org/wiki/Q3806459</t>
         </is>
       </c>
+      <c r="BJ2" t="inlineStr"/>
       <c r="BK2" t="inlineStr"/>
       <c r="BL2" t="inlineStr"/>
       <c r="BM2" t="inlineStr"/>
@@ -970,129 +968,126 @@
       <c r="BO2" t="inlineStr"/>
       <c r="BP2" t="inlineStr"/>
       <c r="BQ2" t="inlineStr"/>
-      <c r="BR2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1980.264.5</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1980.264.5</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
           <t>1980</t>
         </is>
       </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
           <t>Ten-dollar Liberty Head Coin</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Maker</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Christian Gobrecht</t>
+        </is>
+      </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Christian Gobrecht</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
           <t>1785–1844</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr">
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr">
         <is>
           <t>Gobrecht, Christian</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>1785</t>
+        </is>
+      </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>1785</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
           <t>1844</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>https://www.wikidata.org/wiki/Q5109648</t>
+        </is>
+      </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>https://www.wikidata.org/wiki/Q5109648</t>
+          <t>http://vocab.getty.edu/page/ulan/500077295</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500077295</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
           <t>1901</t>
         </is>
+      </c>
+      <c r="AD3" t="n">
+        <v>1901</v>
       </c>
       <c r="AE3" t="n">
         <v>1901</v>
       </c>
-      <c r="AF3" t="n">
-        <v>1901</v>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
           <t>Dimensions unavailable</t>
         </is>
       </c>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr">
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr">
         <is>
           <t>Gift of Heinz L. Stoppelmann, 1980</t>
         </is>
       </c>
+      <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr"/>
@@ -1106,51 +1101,51 @@
       <c r="AU3" t="inlineStr"/>
       <c r="AV3" t="inlineStr"/>
       <c r="AW3" t="inlineStr"/>
-      <c r="AX3" t="inlineStr"/>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY3" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ3" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA3" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/2</t>
         </is>
       </c>
+      <c r="BA3" t="inlineStr"/>
       <c r="BB3" t="inlineStr"/>
-      <c r="BC3" t="inlineStr"/>
-      <c r="BD3" t="b">
-        <v>0</v>
-      </c>
-      <c r="BE3" t="inlineStr"/>
-      <c r="BF3" t="n">
+      <c r="BC3" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="n">
         <v>1079</v>
       </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>Maker</t>
+        </is>
+      </c>
       <c r="BG3" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Christian Gobrecht</t>
         </is>
       </c>
       <c r="BH3" t="inlineStr">
         <is>
-          <t>Christian Gobrecht</t>
+          <t>http://vocab.getty.edu/page/ulan/500077295</t>
         </is>
       </c>
       <c r="BI3" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500077295</t>
-        </is>
-      </c>
-      <c r="BJ3" t="inlineStr">
-        <is>
           <t>https://www.wikidata.org/wiki/Q5109648</t>
         </is>
       </c>
+      <c r="BJ3" t="inlineStr"/>
       <c r="BK3" t="inlineStr"/>
       <c r="BL3" t="inlineStr"/>
       <c r="BM3" t="inlineStr"/>
@@ -1158,53 +1153,50 @@
       <c r="BO3" t="inlineStr"/>
       <c r="BP3" t="inlineStr"/>
       <c r="BQ3" t="inlineStr"/>
-      <c r="BR3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>67.265.9</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>67.265.9</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
           <t>1967</t>
         </is>
       </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
           <t>Two-and-a-Half Dollar Coin</t>
         </is>
       </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
@@ -1221,34 +1213,34 @@
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="inlineStr">
+      <c r="AC4" t="inlineStr">
         <is>
           <t>1909–27</t>
         </is>
       </c>
+      <c r="AD4" t="n">
+        <v>1909</v>
+      </c>
       <c r="AE4" t="n">
-        <v>1909</v>
-      </c>
-      <c r="AF4" t="n">
         <v>1927</v>
       </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
+      </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
           <t>Diam. 11/16 in. (1.7 cm)</t>
         </is>
       </c>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="inlineStr">
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr">
         <is>
           <t>Gift of C. Ruxton Love Jr., 1967</t>
         </is>
       </c>
+      <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="inlineStr"/>
       <c r="AM4" t="inlineStr"/>
@@ -1262,27 +1254,27 @@
       <c r="AU4" t="inlineStr"/>
       <c r="AV4" t="inlineStr"/>
       <c r="AW4" t="inlineStr"/>
-      <c r="AX4" t="inlineStr"/>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY4" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ4" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA4" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/3</t>
         </is>
       </c>
+      <c r="BA4" t="inlineStr"/>
       <c r="BB4" t="inlineStr"/>
-      <c r="BC4" t="inlineStr"/>
-      <c r="BD4" t="b">
-        <v>0</v>
-      </c>
+      <c r="BC4" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD4" t="inlineStr"/>
       <c r="BE4" t="inlineStr"/>
       <c r="BF4" t="inlineStr"/>
       <c r="BG4" t="inlineStr"/>
@@ -1290,71 +1282,68 @@
       <c r="BI4" t="inlineStr"/>
       <c r="BJ4" t="inlineStr"/>
       <c r="BK4" t="inlineStr"/>
-      <c r="BL4" t="inlineStr"/>
+      <c r="BL4" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM4" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN4" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO4" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.7463}</t>
         </is>
       </c>
+      <c r="BO4" t="inlineStr"/>
       <c r="BP4" t="inlineStr"/>
       <c r="BQ4" t="inlineStr"/>
-      <c r="BR4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="b">
-        <v>0</v>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>67.265.10</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>67.265.10</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
           <t>1967</t>
         </is>
       </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
           <t>Two-and-a-Half Dollar Coin</t>
         </is>
       </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
@@ -1371,34 +1360,34 @@
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="inlineStr">
+      <c r="AC5" t="inlineStr">
         <is>
           <t>1909–27</t>
         </is>
       </c>
+      <c r="AD5" t="n">
+        <v>1909</v>
+      </c>
       <c r="AE5" t="n">
-        <v>1909</v>
-      </c>
-      <c r="AF5" t="n">
         <v>1927</v>
       </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
+      </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
           <t>Diam. 11/16 in. (1.7 cm)</t>
         </is>
       </c>
-      <c r="AI5" t="inlineStr"/>
-      <c r="AJ5" t="inlineStr">
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr">
         <is>
           <t>Gift of C. Ruxton Love Jr., 1967</t>
         </is>
       </c>
+      <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="inlineStr"/>
       <c r="AL5" t="inlineStr"/>
       <c r="AM5" t="inlineStr"/>
@@ -1412,27 +1401,27 @@
       <c r="AU5" t="inlineStr"/>
       <c r="AV5" t="inlineStr"/>
       <c r="AW5" t="inlineStr"/>
-      <c r="AX5" t="inlineStr"/>
+      <c r="AX5" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY5" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ5" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA5" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/4</t>
         </is>
       </c>
+      <c r="BA5" t="inlineStr"/>
       <c r="BB5" t="inlineStr"/>
-      <c r="BC5" t="inlineStr"/>
-      <c r="BD5" t="b">
-        <v>0</v>
-      </c>
+      <c r="BC5" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD5" t="inlineStr"/>
       <c r="BE5" t="inlineStr"/>
       <c r="BF5" t="inlineStr"/>
       <c r="BG5" t="inlineStr"/>
@@ -1440,71 +1429,68 @@
       <c r="BI5" t="inlineStr"/>
       <c r="BJ5" t="inlineStr"/>
       <c r="BK5" t="inlineStr"/>
-      <c r="BL5" t="inlineStr"/>
+      <c r="BL5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM5" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN5" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO5" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.7463}</t>
         </is>
       </c>
+      <c r="BO5" t="inlineStr"/>
       <c r="BP5" t="inlineStr"/>
       <c r="BQ5" t="inlineStr"/>
-      <c r="BR5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="b">
-        <v>0</v>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>67.265.11</t>
+        </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>67.265.11</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
           <t>1967</t>
         </is>
       </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
           <t>Two-and-a-Half Dollar Coin</t>
         </is>
       </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
@@ -1521,34 +1507,34 @@
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="inlineStr">
+      <c r="AC6" t="inlineStr">
         <is>
           <t>1909–27</t>
         </is>
       </c>
+      <c r="AD6" t="n">
+        <v>1909</v>
+      </c>
       <c r="AE6" t="n">
-        <v>1909</v>
-      </c>
-      <c r="AF6" t="n">
         <v>1927</v>
       </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
+      </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
           <t>Diam. 11/16 in. (1.7 cm)</t>
         </is>
       </c>
-      <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="inlineStr">
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr">
         <is>
           <t>Gift of C. Ruxton Love Jr., 1967</t>
         </is>
       </c>
+      <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="inlineStr"/>
       <c r="AL6" t="inlineStr"/>
       <c r="AM6" t="inlineStr"/>
@@ -1562,27 +1548,27 @@
       <c r="AU6" t="inlineStr"/>
       <c r="AV6" t="inlineStr"/>
       <c r="AW6" t="inlineStr"/>
-      <c r="AX6" t="inlineStr"/>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY6" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ6" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA6" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/5</t>
         </is>
       </c>
+      <c r="BA6" t="inlineStr"/>
       <c r="BB6" t="inlineStr"/>
-      <c r="BC6" t="inlineStr"/>
-      <c r="BD6" t="b">
-        <v>0</v>
-      </c>
+      <c r="BC6" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD6" t="inlineStr"/>
       <c r="BE6" t="inlineStr"/>
       <c r="BF6" t="inlineStr"/>
       <c r="BG6" t="inlineStr"/>
@@ -1590,71 +1576,68 @@
       <c r="BI6" t="inlineStr"/>
       <c r="BJ6" t="inlineStr"/>
       <c r="BK6" t="inlineStr"/>
-      <c r="BL6" t="inlineStr"/>
+      <c r="BL6" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM6" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN6" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO6" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.7463}</t>
         </is>
       </c>
+      <c r="BO6" t="inlineStr"/>
       <c r="BP6" t="inlineStr"/>
       <c r="BQ6" t="inlineStr"/>
-      <c r="BR6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="b">
-        <v>0</v>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>67.265.12</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>67.265.12</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
           <t>1967</t>
         </is>
       </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
           <t>Two-and-a-Half Dollar Coin</t>
         </is>
       </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -1671,34 +1654,34 @@
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="inlineStr"/>
-      <c r="AD7" t="inlineStr">
+      <c r="AC7" t="inlineStr">
         <is>
           <t>1909–27</t>
         </is>
       </c>
+      <c r="AD7" t="n">
+        <v>1909</v>
+      </c>
       <c r="AE7" t="n">
-        <v>1909</v>
-      </c>
-      <c r="AF7" t="n">
         <v>1927</v>
       </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
+      </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH7" t="inlineStr">
-        <is>
           <t>Diam. 11/16 in. (1.7 cm)</t>
         </is>
       </c>
-      <c r="AI7" t="inlineStr"/>
-      <c r="AJ7" t="inlineStr">
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr">
         <is>
           <t>Gift of C. Ruxton Love Jr., 1967</t>
         </is>
       </c>
+      <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="inlineStr"/>
       <c r="AM7" t="inlineStr"/>
@@ -1712,27 +1695,27 @@
       <c r="AU7" t="inlineStr"/>
       <c r="AV7" t="inlineStr"/>
       <c r="AW7" t="inlineStr"/>
-      <c r="AX7" t="inlineStr"/>
+      <c r="AX7" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY7" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ7" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA7" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/6</t>
         </is>
       </c>
+      <c r="BA7" t="inlineStr"/>
       <c r="BB7" t="inlineStr"/>
-      <c r="BC7" t="inlineStr"/>
-      <c r="BD7" t="b">
-        <v>0</v>
-      </c>
+      <c r="BC7" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD7" t="inlineStr"/>
       <c r="BE7" t="inlineStr"/>
       <c r="BF7" t="inlineStr"/>
       <c r="BG7" t="inlineStr"/>
@@ -1740,71 +1723,68 @@
       <c r="BI7" t="inlineStr"/>
       <c r="BJ7" t="inlineStr"/>
       <c r="BK7" t="inlineStr"/>
-      <c r="BL7" t="inlineStr"/>
+      <c r="BL7" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM7" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN7" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO7" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.7463}</t>
         </is>
       </c>
+      <c r="BO7" t="inlineStr"/>
       <c r="BP7" t="inlineStr"/>
       <c r="BQ7" t="inlineStr"/>
-      <c r="BR7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="C8" t="b">
-        <v>0</v>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>67.265.13</t>
+        </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>67.265.13</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
           <t>1967</t>
         </is>
       </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
           <t>Two-and-a-Half Dollar Coin</t>
         </is>
       </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
@@ -1821,34 +1801,34 @@
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="inlineStr">
+      <c r="AC8" t="inlineStr">
         <is>
           <t>1909–27</t>
         </is>
       </c>
+      <c r="AD8" t="n">
+        <v>1909</v>
+      </c>
       <c r="AE8" t="n">
-        <v>1909</v>
-      </c>
-      <c r="AF8" t="n">
         <v>1927</v>
       </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
+      </c>
       <c r="AG8" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH8" t="inlineStr">
-        <is>
           <t>Diam. 11/16 in. (1.7 cm)</t>
         </is>
       </c>
-      <c r="AI8" t="inlineStr"/>
-      <c r="AJ8" t="inlineStr">
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr">
         <is>
           <t>Gift of C. Ruxton Love Jr., 1967</t>
         </is>
       </c>
+      <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="inlineStr"/>
       <c r="AL8" t="inlineStr"/>
       <c r="AM8" t="inlineStr"/>
@@ -1862,27 +1842,27 @@
       <c r="AU8" t="inlineStr"/>
       <c r="AV8" t="inlineStr"/>
       <c r="AW8" t="inlineStr"/>
-      <c r="AX8" t="inlineStr"/>
+      <c r="AX8" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY8" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ8" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA8" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/7</t>
         </is>
       </c>
+      <c r="BA8" t="inlineStr"/>
       <c r="BB8" t="inlineStr"/>
-      <c r="BC8" t="inlineStr"/>
-      <c r="BD8" t="b">
-        <v>0</v>
-      </c>
+      <c r="BC8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD8" t="inlineStr"/>
       <c r="BE8" t="inlineStr"/>
       <c r="BF8" t="inlineStr"/>
       <c r="BG8" t="inlineStr"/>
@@ -1890,83 +1870,80 @@
       <c r="BI8" t="inlineStr"/>
       <c r="BJ8" t="inlineStr"/>
       <c r="BK8" t="inlineStr"/>
-      <c r="BL8" t="inlineStr"/>
+      <c r="BL8" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM8" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN8" t="inlineStr">
         <is>
-          <t>Object diameter</t>
+          <t>{'Diameter': 1.7463}</t>
         </is>
       </c>
       <c r="BO8" t="inlineStr">
         <is>
-          <t>{'Diameter': 1.7463}</t>
+          <t>Coins</t>
         </is>
       </c>
       <c r="BP8" t="inlineStr">
         <is>
-          <t>Coins</t>
+          <t>http://vocab.getty.edu/page/aat/300037222</t>
         </is>
       </c>
       <c r="BQ8" t="inlineStr">
-        <is>
-          <t>http://vocab.getty.edu/page/aat/300037222</t>
-        </is>
-      </c>
-      <c r="BR8" t="inlineStr">
         <is>
           <t>https://www.wikidata.org/wiki/Q41207</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="C9" t="b">
-        <v>0</v>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>67.265.14</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>67.265.14</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
           <t>1967</t>
         </is>
       </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
           <t>Two-and-a-Half Dollar Coin</t>
         </is>
       </c>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
@@ -1983,34 +1960,34 @@
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr">
+      <c r="AC9" t="inlineStr">
         <is>
           <t>1909–27</t>
         </is>
       </c>
+      <c r="AD9" t="n">
+        <v>1909</v>
+      </c>
       <c r="AE9" t="n">
-        <v>1909</v>
-      </c>
-      <c r="AF9" t="n">
         <v>1927</v>
       </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
+      </c>
       <c r="AG9" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH9" t="inlineStr">
-        <is>
           <t>Diam. 11/16 in. (1.7 cm)</t>
         </is>
       </c>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="inlineStr">
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr">
         <is>
           <t>Gift of C. Ruxton Love Jr., 1967</t>
         </is>
       </c>
+      <c r="AJ9" t="inlineStr"/>
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
@@ -2024,27 +2001,27 @@
       <c r="AU9" t="inlineStr"/>
       <c r="AV9" t="inlineStr"/>
       <c r="AW9" t="inlineStr"/>
-      <c r="AX9" t="inlineStr"/>
+      <c r="AX9" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY9" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ9" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA9" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/8</t>
         </is>
       </c>
+      <c r="BA9" t="inlineStr"/>
       <c r="BB9" t="inlineStr"/>
-      <c r="BC9" t="inlineStr"/>
-      <c r="BD9" t="b">
-        <v>0</v>
-      </c>
+      <c r="BC9" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD9" t="inlineStr"/>
       <c r="BE9" t="inlineStr"/>
       <c r="BF9" t="inlineStr"/>
       <c r="BG9" t="inlineStr"/>
@@ -2052,83 +2029,80 @@
       <c r="BI9" t="inlineStr"/>
       <c r="BJ9" t="inlineStr"/>
       <c r="BK9" t="inlineStr"/>
-      <c r="BL9" t="inlineStr"/>
+      <c r="BL9" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM9" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN9" t="inlineStr">
         <is>
-          <t>Object diameter</t>
+          <t>{'Diameter': 1.7463}</t>
         </is>
       </c>
       <c r="BO9" t="inlineStr">
         <is>
-          <t>{'Diameter': 1.7463}</t>
+          <t>Eagles</t>
         </is>
       </c>
       <c r="BP9" t="inlineStr">
         <is>
-          <t>Eagles</t>
+          <t>http://vocab.getty.edu/page/aat/300250049</t>
         </is>
       </c>
       <c r="BQ9" t="inlineStr">
-        <is>
-          <t>http://vocab.getty.edu/page/aat/300250049</t>
-        </is>
-      </c>
-      <c r="BR9" t="inlineStr">
         <is>
           <t>https://www.wikidata.org/wiki/Q2092297</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="C10" t="b">
-        <v>0</v>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>67.265.15</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>67.265.15</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
           <t>1967</t>
         </is>
       </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
           <t>Two-and-a-Half Dollar Coin</t>
         </is>
       </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -2145,34 +2119,34 @@
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="inlineStr">
+      <c r="AC10" t="inlineStr">
         <is>
           <t>1909–27</t>
         </is>
       </c>
+      <c r="AD10" t="n">
+        <v>1909</v>
+      </c>
       <c r="AE10" t="n">
-        <v>1909</v>
-      </c>
-      <c r="AF10" t="n">
         <v>1927</v>
       </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
+      </c>
       <c r="AG10" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH10" t="inlineStr">
-        <is>
           <t>Diam. 11/16 in. (1.7 cm)</t>
         </is>
       </c>
-      <c r="AI10" t="inlineStr"/>
-      <c r="AJ10" t="inlineStr">
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr">
         <is>
           <t>Gift of C. Ruxton Love Jr., 1967</t>
         </is>
       </c>
+      <c r="AJ10" t="inlineStr"/>
       <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="inlineStr"/>
       <c r="AM10" t="inlineStr"/>
@@ -2186,27 +2160,27 @@
       <c r="AU10" t="inlineStr"/>
       <c r="AV10" t="inlineStr"/>
       <c r="AW10" t="inlineStr"/>
-      <c r="AX10" t="inlineStr"/>
+      <c r="AX10" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY10" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ10" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA10" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/9</t>
         </is>
       </c>
+      <c r="BA10" t="inlineStr"/>
       <c r="BB10" t="inlineStr"/>
-      <c r="BC10" t="inlineStr"/>
-      <c r="BD10" t="b">
-        <v>0</v>
-      </c>
+      <c r="BC10" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD10" t="inlineStr"/>
       <c r="BE10" t="inlineStr"/>
       <c r="BF10" t="inlineStr"/>
       <c r="BG10" t="inlineStr"/>
@@ -2214,147 +2188,144 @@
       <c r="BI10" t="inlineStr"/>
       <c r="BJ10" t="inlineStr"/>
       <c r="BK10" t="inlineStr"/>
-      <c r="BL10" t="inlineStr"/>
+      <c r="BL10" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM10" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN10" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO10" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.7463}</t>
         </is>
       </c>
+      <c r="BO10" t="inlineStr"/>
       <c r="BP10" t="inlineStr"/>
       <c r="BQ10" t="inlineStr"/>
-      <c r="BR10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1979.486.3</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1979.486.3</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
           <t>1979</t>
         </is>
       </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
           <t>Two-and-a-half-dollar Indian Head Coin</t>
         </is>
       </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>Maker</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Bela Lyon Pratt</t>
+        </is>
+      </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>Bela Lyon Pratt</t>
-        </is>
-      </c>
-      <c r="U11" t="inlineStr">
-        <is>
           <t>1867–1917</t>
         </is>
       </c>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr">
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr">
         <is>
           <t>Pratt, Bela Lyon</t>
         </is>
       </c>
-      <c r="X11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>1867</t>
+        </is>
+      </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>1867</t>
-        </is>
-      </c>
-      <c r="Z11" t="inlineStr">
-        <is>
           <t>1917</t>
         </is>
       </c>
-      <c r="AA11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>https://www.wikidata.org/wiki/Q4881787</t>
+        </is>
+      </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>https://www.wikidata.org/wiki/Q4881787</t>
+          <t>http://vocab.getty.edu/page/ulan/500095555</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500095555</t>
-        </is>
-      </c>
-      <c r="AD11" t="inlineStr">
-        <is>
           <t>1912</t>
         </is>
+      </c>
+      <c r="AD11" t="n">
+        <v>1912</v>
       </c>
       <c r="AE11" t="n">
         <v>1912</v>
       </c>
-      <c r="AF11" t="n">
-        <v>1912</v>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
       </c>
       <c r="AG11" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH11" t="inlineStr">
-        <is>
           <t>Dimensions unavailable</t>
         </is>
       </c>
-      <c r="AI11" t="inlineStr"/>
-      <c r="AJ11" t="inlineStr">
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr">
         <is>
           <t>Gift of Heinz L. Stoppelmann, 1979</t>
         </is>
       </c>
+      <c r="AJ11" t="inlineStr"/>
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="inlineStr"/>
       <c r="AM11" t="inlineStr"/>
@@ -2368,193 +2339,190 @@
       <c r="AU11" t="inlineStr"/>
       <c r="AV11" t="inlineStr"/>
       <c r="AW11" t="inlineStr"/>
-      <c r="AX11" t="inlineStr"/>
+      <c r="AX11" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY11" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ11" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA11" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/10</t>
         </is>
       </c>
+      <c r="BA11" t="inlineStr"/>
       <c r="BB11" t="inlineStr"/>
-      <c r="BC11" t="inlineStr"/>
-      <c r="BD11" t="b">
-        <v>0</v>
-      </c>
-      <c r="BE11" t="inlineStr"/>
-      <c r="BF11" t="n">
+      <c r="BC11" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD11" t="inlineStr"/>
+      <c r="BE11" t="n">
         <v>1080</v>
       </c>
+      <c r="BF11" t="inlineStr">
+        <is>
+          <t>Maker</t>
+        </is>
+      </c>
       <c r="BG11" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Bela Lyon Pratt</t>
         </is>
       </c>
       <c r="BH11" t="inlineStr">
         <is>
-          <t>Bela Lyon Pratt</t>
+          <t>http://vocab.getty.edu/page/ulan/500095555</t>
         </is>
       </c>
       <c r="BI11" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500095555</t>
-        </is>
-      </c>
-      <c r="BJ11" t="inlineStr">
-        <is>
           <t>https://www.wikidata.org/wiki/Q4881787</t>
         </is>
       </c>
+      <c r="BJ11" t="inlineStr"/>
       <c r="BK11" t="inlineStr"/>
-      <c r="BL11" t="inlineStr"/>
+      <c r="BL11" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM11" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN11" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO11" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.7}</t>
         </is>
       </c>
+      <c r="BO11" t="inlineStr"/>
       <c r="BP11" t="inlineStr"/>
       <c r="BQ11" t="inlineStr"/>
-      <c r="BR11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
+      <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="C12" t="b">
-        <v>0</v>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1979.486.2</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1979.486.2</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
           <t>1979</t>
         </is>
       </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
           <t>Two-and-a-half-dollar Liberty Head Coin</t>
         </is>
       </c>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>Maker</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Christian Gobrecht</t>
+        </is>
+      </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>Christian Gobrecht</t>
-        </is>
-      </c>
-      <c r="U12" t="inlineStr">
-        <is>
           <t>1785–1844</t>
         </is>
       </c>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr">
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr">
         <is>
           <t>Gobrecht, Christian</t>
         </is>
       </c>
-      <c r="X12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>1785</t>
+        </is>
+      </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>1785</t>
-        </is>
-      </c>
-      <c r="Z12" t="inlineStr">
-        <is>
           <t>1844</t>
         </is>
       </c>
-      <c r="AA12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>https://www.wikidata.org/wiki/Q5109648</t>
+        </is>
+      </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>https://www.wikidata.org/wiki/Q5109648</t>
+          <t>http://vocab.getty.edu/page/ulan/500077295</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500077295</t>
-        </is>
-      </c>
-      <c r="AD12" t="inlineStr">
-        <is>
           <t>1907</t>
         </is>
+      </c>
+      <c r="AD12" t="n">
+        <v>1907</v>
       </c>
       <c r="AE12" t="n">
         <v>1907</v>
       </c>
-      <c r="AF12" t="n">
-        <v>1907</v>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
       </c>
       <c r="AG12" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH12" t="inlineStr">
-        <is>
           <t>Dimensions unavailable</t>
         </is>
       </c>
-      <c r="AI12" t="inlineStr"/>
-      <c r="AJ12" t="inlineStr">
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr">
         <is>
           <t>Gift of Heinz L. Stoppelmann, 1979</t>
         </is>
       </c>
+      <c r="AJ12" t="inlineStr"/>
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="inlineStr"/>
@@ -2568,197 +2536,194 @@
       <c r="AU12" t="inlineStr"/>
       <c r="AV12" t="inlineStr"/>
       <c r="AW12" t="inlineStr"/>
-      <c r="AX12" t="inlineStr"/>
+      <c r="AX12" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY12" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ12" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA12" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/11</t>
         </is>
       </c>
+      <c r="BA12" t="inlineStr"/>
       <c r="BB12" t="inlineStr"/>
-      <c r="BC12" t="inlineStr"/>
-      <c r="BD12" t="b">
-        <v>0</v>
-      </c>
-      <c r="BE12" t="inlineStr"/>
-      <c r="BF12" t="n">
+      <c r="BC12" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD12" t="inlineStr"/>
+      <c r="BE12" t="n">
         <v>1079</v>
       </c>
+      <c r="BF12" t="inlineStr">
+        <is>
+          <t>Maker</t>
+        </is>
+      </c>
       <c r="BG12" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Christian Gobrecht</t>
         </is>
       </c>
       <c r="BH12" t="inlineStr">
         <is>
-          <t>Christian Gobrecht</t>
+          <t>http://vocab.getty.edu/page/ulan/500077295</t>
         </is>
       </c>
       <c r="BI12" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500077295</t>
-        </is>
-      </c>
-      <c r="BJ12" t="inlineStr">
-        <is>
           <t>https://www.wikidata.org/wiki/Q5109648</t>
         </is>
       </c>
+      <c r="BJ12" t="inlineStr"/>
       <c r="BK12" t="inlineStr"/>
-      <c r="BL12" t="inlineStr"/>
+      <c r="BL12" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM12" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN12" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO12" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.7}</t>
         </is>
       </c>
+      <c r="BO12" t="inlineStr"/>
       <c r="BP12" t="inlineStr"/>
       <c r="BQ12" t="inlineStr"/>
-      <c r="BR12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
+      <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="C13" t="b">
-        <v>0</v>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1979.486.7</t>
+        </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1979.486.7</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
           <t>1979</t>
         </is>
       </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
           <t>Twenty-dollar Liberty Head Coin</t>
         </is>
       </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>Maker</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>James Barton Longacre</t>
+        </is>
+      </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>James Barton Longacre</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr">
-        <is>
           <t>American, Delaware County, Pennsylvania 1794–1869 Philadelphia, Pennsylvania</t>
         </is>
       </c>
-      <c r="V13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Longacre, James Barton</t>
+        </is>
+      </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>Longacre, James Barton</t>
+          <t>American</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>American</t>
+          <t>1794</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>1794</t>
-        </is>
-      </c>
-      <c r="Z13" t="inlineStr">
-        <is>
           <t>1869</t>
         </is>
       </c>
-      <c r="AA13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>https://www.wikidata.org/wiki/Q3806459</t>
+        </is>
+      </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>https://www.wikidata.org/wiki/Q3806459</t>
+          <t>http://vocab.getty.edu/page/ulan/500011409</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500011409</t>
-        </is>
-      </c>
-      <c r="AD13" t="inlineStr">
-        <is>
           <t>1876</t>
         </is>
+      </c>
+      <c r="AD13" t="n">
+        <v>1876</v>
       </c>
       <c r="AE13" t="n">
         <v>1876</v>
       </c>
-      <c r="AF13" t="n">
-        <v>1876</v>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
       </c>
       <c r="AG13" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH13" t="inlineStr">
-        <is>
           <t>Dimensions unavailable</t>
         </is>
       </c>
-      <c r="AI13" t="inlineStr"/>
-      <c r="AJ13" t="inlineStr">
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr">
         <is>
           <t>Gift of Heinz L. Stoppelmann, 1979</t>
         </is>
       </c>
+      <c r="AJ13" t="inlineStr"/>
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr"/>
       <c r="AM13" t="inlineStr"/>
@@ -2772,193 +2737,190 @@
       <c r="AU13" t="inlineStr"/>
       <c r="AV13" t="inlineStr"/>
       <c r="AW13" t="inlineStr"/>
-      <c r="AX13" t="inlineStr"/>
+      <c r="AX13" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY13" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ13" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA13" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/12</t>
         </is>
       </c>
+      <c r="BA13" t="inlineStr"/>
       <c r="BB13" t="inlineStr"/>
-      <c r="BC13" t="inlineStr"/>
-      <c r="BD13" t="b">
-        <v>0</v>
-      </c>
-      <c r="BE13" t="inlineStr"/>
-      <c r="BF13" t="n">
+      <c r="BC13" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD13" t="inlineStr"/>
+      <c r="BE13" t="n">
         <v>164292</v>
       </c>
+      <c r="BF13" t="inlineStr">
+        <is>
+          <t>Maker</t>
+        </is>
+      </c>
       <c r="BG13" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>James Barton Longacre</t>
         </is>
       </c>
       <c r="BH13" t="inlineStr">
         <is>
-          <t>James Barton Longacre</t>
+          <t>http://vocab.getty.edu/page/ulan/500011409</t>
         </is>
       </c>
       <c r="BI13" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500011409</t>
-        </is>
-      </c>
-      <c r="BJ13" t="inlineStr">
-        <is>
           <t>https://www.wikidata.org/wiki/Q3806459</t>
         </is>
       </c>
+      <c r="BJ13" t="inlineStr"/>
       <c r="BK13" t="inlineStr"/>
-      <c r="BL13" t="inlineStr"/>
+      <c r="BL13" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM13" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN13" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO13" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.7}</t>
         </is>
       </c>
+      <c r="BO13" t="inlineStr"/>
       <c r="BP13" t="inlineStr"/>
       <c r="BQ13" t="inlineStr"/>
-      <c r="BR13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
+      <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="C14" t="b">
-        <v>0</v>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1979.486.4</t>
+        </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1979.486.4</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
           <t>1979</t>
         </is>
       </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
           <t>Five-dollar Indian Head Coin</t>
         </is>
       </c>
+      <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>Maker</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Bela Lyon Pratt</t>
+        </is>
+      </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>Bela Lyon Pratt</t>
-        </is>
-      </c>
-      <c r="U14" t="inlineStr">
-        <is>
           <t>1867–1917</t>
         </is>
       </c>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr">
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr">
         <is>
           <t>Pratt, Bela Lyon</t>
         </is>
       </c>
-      <c r="X14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>1867</t>
+        </is>
+      </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>1867</t>
-        </is>
-      </c>
-      <c r="Z14" t="inlineStr">
-        <is>
           <t>1917</t>
         </is>
       </c>
-      <c r="AA14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>https://www.wikidata.org/wiki/Q4881787</t>
+        </is>
+      </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>https://www.wikidata.org/wiki/Q4881787</t>
+          <t>http://vocab.getty.edu/page/ulan/500095555</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500095555</t>
-        </is>
-      </c>
-      <c r="AD14" t="inlineStr">
-        <is>
           <t>1910</t>
         </is>
+      </c>
+      <c r="AD14" t="n">
+        <v>1910</v>
       </c>
       <c r="AE14" t="n">
         <v>1910</v>
       </c>
-      <c r="AF14" t="n">
-        <v>1910</v>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
       </c>
       <c r="AG14" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH14" t="inlineStr">
-        <is>
           <t>Dimensions unavailable</t>
         </is>
       </c>
-      <c r="AI14" t="inlineStr"/>
-      <c r="AJ14" t="inlineStr">
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr">
         <is>
           <t>Gift of Heinz L. Stoppelmann, 1979</t>
         </is>
       </c>
+      <c r="AJ14" t="inlineStr"/>
       <c r="AK14" t="inlineStr"/>
       <c r="AL14" t="inlineStr"/>
       <c r="AM14" t="inlineStr"/>
@@ -2972,193 +2934,190 @@
       <c r="AU14" t="inlineStr"/>
       <c r="AV14" t="inlineStr"/>
       <c r="AW14" t="inlineStr"/>
-      <c r="AX14" t="inlineStr"/>
+      <c r="AX14" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY14" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ14" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA14" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/13</t>
         </is>
       </c>
+      <c r="BA14" t="inlineStr"/>
       <c r="BB14" t="inlineStr"/>
-      <c r="BC14" t="inlineStr"/>
-      <c r="BD14" t="b">
-        <v>0</v>
-      </c>
-      <c r="BE14" t="inlineStr"/>
-      <c r="BF14" t="n">
+      <c r="BC14" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD14" t="inlineStr"/>
+      <c r="BE14" t="n">
         <v>1080</v>
       </c>
+      <c r="BF14" t="inlineStr">
+        <is>
+          <t>Maker</t>
+        </is>
+      </c>
       <c r="BG14" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Bela Lyon Pratt</t>
         </is>
       </c>
       <c r="BH14" t="inlineStr">
         <is>
-          <t>Bela Lyon Pratt</t>
+          <t>http://vocab.getty.edu/page/ulan/500095555</t>
         </is>
       </c>
       <c r="BI14" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500095555</t>
-        </is>
-      </c>
-      <c r="BJ14" t="inlineStr">
-        <is>
           <t>https://www.wikidata.org/wiki/Q4881787</t>
         </is>
       </c>
+      <c r="BJ14" t="inlineStr"/>
       <c r="BK14" t="inlineStr"/>
-      <c r="BL14" t="inlineStr"/>
+      <c r="BL14" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM14" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN14" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO14" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.7}</t>
         </is>
       </c>
+      <c r="BO14" t="inlineStr"/>
       <c r="BP14" t="inlineStr"/>
       <c r="BQ14" t="inlineStr"/>
-      <c r="BR14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
+      <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="C15" t="b">
-        <v>0</v>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1979.486.5</t>
+        </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1979.486.5</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
           <t>1979</t>
         </is>
       </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Coin</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
           <t>Five-dollar Liberty Head Coin</t>
         </is>
       </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>Maker</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Christian Gobrecht</t>
+        </is>
+      </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>Christian Gobrecht</t>
-        </is>
-      </c>
-      <c r="U15" t="inlineStr">
-        <is>
           <t>1785–1844</t>
         </is>
       </c>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr">
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr">
         <is>
           <t>Gobrecht, Christian</t>
         </is>
       </c>
-      <c r="X15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>1785</t>
+        </is>
+      </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>1785</t>
-        </is>
-      </c>
-      <c r="Z15" t="inlineStr">
-        <is>
           <t>1844</t>
         </is>
       </c>
-      <c r="AA15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>https://www.wikidata.org/wiki/Q5109648</t>
+        </is>
+      </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>https://www.wikidata.org/wiki/Q5109648</t>
+          <t>http://vocab.getty.edu/page/ulan/500077295</t>
         </is>
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500077295</t>
-        </is>
-      </c>
-      <c r="AD15" t="inlineStr">
-        <is>
           <t>1907</t>
         </is>
+      </c>
+      <c r="AD15" t="n">
+        <v>1907</v>
       </c>
       <c r="AE15" t="n">
         <v>1907</v>
       </c>
-      <c r="AF15" t="n">
-        <v>1907</v>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
       </c>
       <c r="AG15" t="inlineStr">
         <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="AH15" t="inlineStr">
-        <is>
           <t>Dimensions unavailable</t>
         </is>
       </c>
-      <c r="AI15" t="inlineStr"/>
-      <c r="AJ15" t="inlineStr">
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="inlineStr">
         <is>
           <t>Gift of Heinz L. Stoppelmann, 1979</t>
         </is>
       </c>
+      <c r="AJ15" t="inlineStr"/>
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
@@ -3172,122 +3131,119 @@
       <c r="AU15" t="inlineStr"/>
       <c r="AV15" t="inlineStr"/>
       <c r="AW15" t="inlineStr"/>
-      <c r="AX15" t="inlineStr"/>
+      <c r="AX15" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY15" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ15" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA15" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/14</t>
         </is>
       </c>
+      <c r="BA15" t="inlineStr"/>
       <c r="BB15" t="inlineStr"/>
-      <c r="BC15" t="inlineStr"/>
-      <c r="BD15" t="b">
-        <v>0</v>
-      </c>
-      <c r="BE15" t="inlineStr"/>
-      <c r="BF15" t="n">
+      <c r="BC15" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD15" t="inlineStr"/>
+      <c r="BE15" t="n">
         <v>1079</v>
       </c>
+      <c r="BF15" t="inlineStr">
+        <is>
+          <t>Maker</t>
+        </is>
+      </c>
       <c r="BG15" t="inlineStr">
         <is>
-          <t>Maker</t>
+          <t>Christian Gobrecht</t>
         </is>
       </c>
       <c r="BH15" t="inlineStr">
         <is>
-          <t>Christian Gobrecht</t>
+          <t>http://vocab.getty.edu/page/ulan/500077295</t>
         </is>
       </c>
       <c r="BI15" t="inlineStr">
         <is>
-          <t>http://vocab.getty.edu/page/ulan/500077295</t>
-        </is>
-      </c>
-      <c r="BJ15" t="inlineStr">
-        <is>
           <t>https://www.wikidata.org/wiki/Q5109648</t>
         </is>
       </c>
+      <c r="BJ15" t="inlineStr"/>
       <c r="BK15" t="inlineStr"/>
-      <c r="BL15" t="inlineStr"/>
+      <c r="BL15" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM15" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN15" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO15" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.7}</t>
         </is>
       </c>
+      <c r="BO15" t="inlineStr"/>
       <c r="BP15" t="inlineStr"/>
       <c r="BQ15" t="inlineStr"/>
-      <c r="BR15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
+      <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="C16" t="b">
-        <v>0</v>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>16.74.49</t>
+        </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>16.74.49</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
           <t>1916</t>
         </is>
       </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>The American Wing</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>The American Wing</t>
+          <t>Coin</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Coin</t>
+          <t>Coin, 1/2 Real</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Coin, 1/2 Real</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
           <t>Mexican</t>
         </is>
       </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
@@ -3303,47 +3259,47 @@
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="inlineStr"/>
-      <c r="AD16" t="inlineStr">
+      <c r="AC16" t="inlineStr">
         <is>
           <t>1665–1700</t>
         </is>
       </c>
+      <c r="AD16" t="n">
+        <v>1665</v>
+      </c>
       <c r="AE16" t="n">
-        <v>1665</v>
-      </c>
-      <c r="AF16" t="n">
         <v>1700</v>
       </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>Silver</t>
+        </is>
+      </c>
       <c r="AG16" t="inlineStr">
         <is>
-          <t>Silver</t>
-        </is>
-      </c>
-      <c r="AH16" t="inlineStr">
-        <is>
           <t>Diam. 1/2 in. (1.3 cm)</t>
         </is>
       </c>
-      <c r="AI16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr">
+        <is>
+          <t>Gift of Mrs. Russell Sage, 1916</t>
+        </is>
+      </c>
       <c r="AJ16" t="inlineStr">
         <is>
-          <t>Gift of Mrs. Russell Sage, 1916</t>
-        </is>
-      </c>
-      <c r="AK16" t="inlineStr">
-        <is>
           <t>Made in</t>
         </is>
       </c>
+      <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
-      <c r="AN16" t="inlineStr"/>
-      <c r="AO16" t="inlineStr">
+      <c r="AN16" t="inlineStr">
         <is>
           <t>Mexico</t>
         </is>
       </c>
+      <c r="AO16" t="inlineStr"/>
       <c r="AP16" t="inlineStr"/>
       <c r="AQ16" t="inlineStr"/>
       <c r="AR16" t="inlineStr"/>
@@ -3352,27 +3308,27 @@
       <c r="AU16" t="inlineStr"/>
       <c r="AV16" t="inlineStr"/>
       <c r="AW16" t="inlineStr"/>
-      <c r="AX16" t="inlineStr"/>
+      <c r="AX16" t="inlineStr">
+        <is>
+          <t>2021-04-06T04:41:04.967Z</t>
+        </is>
+      </c>
       <c r="AY16" t="inlineStr">
         <is>
-          <t>2021-04-06T04:41:04.967Z</t>
+          <t>Metropolitan Museum of Art, New York, NY</t>
         </is>
       </c>
       <c r="AZ16" t="inlineStr">
         <is>
-          <t>Metropolitan Museum of Art, New York, NY</t>
-        </is>
-      </c>
-      <c r="BA16" t="inlineStr">
-        <is>
           <t>https://www.metmuseum.org/art/collection/search/15</t>
         </is>
       </c>
+      <c r="BA16" t="inlineStr"/>
       <c r="BB16" t="inlineStr"/>
-      <c r="BC16" t="inlineStr"/>
-      <c r="BD16" t="b">
-        <v>0</v>
-      </c>
+      <c r="BC16" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD16" t="inlineStr"/>
       <c r="BE16" t="inlineStr"/>
       <c r="BF16" t="inlineStr"/>
       <c r="BG16" t="inlineStr"/>
@@ -3380,25 +3336,24 @@
       <c r="BI16" t="inlineStr"/>
       <c r="BJ16" t="inlineStr"/>
       <c r="BK16" t="inlineStr"/>
-      <c r="BL16" t="inlineStr"/>
+      <c r="BL16" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
       <c r="BM16" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Object diameter</t>
         </is>
       </c>
       <c r="BN16" t="inlineStr">
         <is>
-          <t>Object diameter</t>
-        </is>
-      </c>
-      <c r="BO16" t="inlineStr">
-        <is>
           <t>{'Diameter': 1.27}</t>
         </is>
       </c>
+      <c r="BO16" t="inlineStr"/>
       <c r="BP16" t="inlineStr"/>
       <c r="BQ16" t="inlineStr"/>
-      <c r="BR16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>